<commit_message>
kafka teacing rwth paper
</commit_message>
<xml_diff>
--- a/thesis/ukapp2/wqu_isc/pins/Space Database Checks AG.xlsx
+++ b/thesis/ukapp2/wqu_isc/pins/Space Database Checks AG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Dropbox\rtmp\src\org\thesis\ukapp2\wqu_isc\pins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF4A1DD-448E-4306-87D0-8DFA668707F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458C4B73-CCC2-467F-A313-8B67F3BA5937}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1848" yWindow="732" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1069,12 +1069,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="2" t="s">
+    <row r="27" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>35</v>
+      <c r="F27" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>